<commit_message>
Update - Data_Superf_NumZonas included
</commit_message>
<xml_diff>
--- a/DataIn/VarDep/Data_Superf_NumZonas.xlsx
+++ b/DataIn/VarDep/Data_Superf_NumZonas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a6b088a06617d4fb/Ejercicio 7/Documents/Documents/Maestria/Modelado_Merlin/GitHub_Datos/Social_Model_Enchugal/DataIn/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a6b088a06617d4fb/Ejercicio 7/Documents/Documents/Maestria/Modelado_Merlin/GitHub_Datos/Social_Model_Enchugal/DataIn/VarDep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{50E3BE36-696C-4F83-981A-B305DA2E3B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{113CADEA-F1EE-4E1D-96D6-1777FA1DD7E3}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{50E3BE36-696C-4F83-981A-B305DA2E3B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{519AB427-62D1-4C1F-860D-AED66CCA774B}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2640" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="264">
   <si>
     <t>Alaba</t>
   </si>
@@ -642,6 +642,180 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>Antonio Mbunh</t>
+  </si>
+  <si>
+    <t>Bulna Ntumba</t>
+  </si>
+  <si>
+    <t>Nghala Pungana</t>
+  </si>
+  <si>
+    <t>Samba Ndum</t>
+  </si>
+  <si>
+    <t>Tomas Isnaba</t>
+  </si>
+  <si>
+    <t>Viriato Quintunda</t>
+  </si>
+  <si>
+    <t>Bunhna Iamta</t>
+  </si>
+  <si>
+    <t>Clautche Ndami</t>
+  </si>
+  <si>
+    <t>Tamba Ndami</t>
+  </si>
+  <si>
+    <t>Buan Castigo</t>
+  </si>
+  <si>
+    <t>Cumsana Yala</t>
+  </si>
+  <si>
+    <t>Futana Cabi</t>
+  </si>
+  <si>
+    <t>Eusebio Ncanha</t>
+  </si>
+  <si>
+    <t>Wangna Ntchoba</t>
+  </si>
+  <si>
+    <t>Bifule Winaba</t>
+  </si>
+  <si>
+    <t>Dan Natelna</t>
+  </si>
+  <si>
+    <t>Nghala Diuai</t>
+  </si>
+  <si>
+    <t>Sangueia Blaque</t>
+  </si>
+  <si>
+    <t>Winaba Ndongle</t>
+  </si>
+  <si>
+    <t>Djone Bidagle</t>
+  </si>
+  <si>
+    <t>Ncahota Nghala</t>
+  </si>
+  <si>
+    <t>Nhudna Pansau</t>
+  </si>
+  <si>
+    <t>Ntrum Ncanha</t>
+  </si>
+  <si>
+    <t>Marate Man</t>
+  </si>
+  <si>
+    <t>Bigna Fonseca</t>
+  </si>
+  <si>
+    <t>Bitique Biem</t>
+  </si>
+  <si>
+    <t>Bringpande Bidane</t>
+  </si>
+  <si>
+    <t>Catchna Man</t>
+  </si>
+  <si>
+    <t>Quissifqueia Mbana</t>
+  </si>
+  <si>
+    <t>Tibna Maiaco</t>
+  </si>
+  <si>
+    <t>Artur Buassa</t>
+  </si>
+  <si>
+    <t>Bique Bedamite</t>
+  </si>
+  <si>
+    <t>Cul Tchongo</t>
+  </si>
+  <si>
+    <t>Aiace Quior</t>
+  </si>
+  <si>
+    <t>Ncassumba Filif</t>
+  </si>
+  <si>
+    <t>Nghotmara Filif</t>
+  </si>
+  <si>
+    <t>Sumfone Tagadad</t>
+  </si>
+  <si>
+    <t>Tamble Cunhate</t>
+  </si>
+  <si>
+    <t>Quifuc Pan</t>
+  </si>
+  <si>
+    <t>Midana Fidaiba</t>
+  </si>
+  <si>
+    <t>Rungna Yala</t>
+  </si>
+  <si>
+    <t>Birabotcha Togna</t>
+  </si>
+  <si>
+    <t>Marate Isnaba</t>
+  </si>
+  <si>
+    <t>Calabus Quintunda</t>
+  </si>
+  <si>
+    <t>Tugna Quintunda</t>
+  </si>
+  <si>
+    <t>Inma Cabi</t>
+  </si>
+  <si>
+    <t>Pangueia Tus</t>
+  </si>
+  <si>
+    <t>Matchna Sambu</t>
+  </si>
+  <si>
+    <t>Nquissande Siuna</t>
+  </si>
+  <si>
+    <t>Americano Mbunde</t>
+  </si>
+  <si>
+    <t>Bicamtala Ntumba</t>
+  </si>
+  <si>
+    <t>Fogna Siga</t>
+  </si>
+  <si>
+    <t>Domingos Sincar</t>
+  </si>
+  <si>
+    <t>Biaun Wangna</t>
+  </si>
+  <si>
+    <t>Cletche Togna</t>
+  </si>
+  <si>
+    <t>Bigna Man</t>
+  </si>
+  <si>
+    <t>Binhanarem Isnaba</t>
+  </si>
+  <si>
+    <t>Augusto Sumba</t>
   </si>
 </sst>
 </file>
@@ -677,7 +851,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -753,6 +927,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -912,7 +1092,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -946,6 +1126,8 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3509,8 +3691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{487958FD-D8FC-4126-AEA0-A944EA1E8DB9}">
   <dimension ref="A1:C131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection sqref="A1:A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3521,7 +3703,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="27" t="s">
         <v>205</v>
       </c>
       <c r="B1" s="24" t="s">
@@ -3532,8 +3714,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>70</v>
+      <c r="A2" s="28" t="s">
+        <v>206</v>
       </c>
       <c r="B2" s="23">
         <v>1.9217</v>
@@ -3543,8 +3725,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
-        <v>185</v>
+      <c r="A3" s="28" t="s">
+        <v>207</v>
       </c>
       <c r="B3" s="23">
         <v>1.8387000000000002</v>
@@ -3554,8 +3736,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>18</v>
+      <c r="A4" s="28" t="s">
+        <v>208</v>
       </c>
       <c r="B4" s="23">
         <v>1.6564000000000001</v>
@@ -3565,8 +3747,8 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
-        <v>25</v>
+      <c r="A5" s="28" t="s">
+        <v>209</v>
       </c>
       <c r="B5" s="23">
         <v>2.6717</v>
@@ -3576,8 +3758,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
-        <v>5</v>
+      <c r="A6" s="28" t="s">
+        <v>210</v>
       </c>
       <c r="B6" s="23">
         <v>2.2281</v>
@@ -3587,8 +3769,8 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
-        <v>198</v>
+      <c r="A7" s="28" t="s">
+        <v>211</v>
       </c>
       <c r="B7" s="23">
         <v>5.3822999999999999</v>
@@ -3598,7 +3780,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="28" t="s">
         <v>158</v>
       </c>
       <c r="B8" s="23">
@@ -3609,7 +3791,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="28" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="23">
@@ -3620,8 +3802,8 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>30</v>
+      <c r="A10" s="28" t="s">
+        <v>212</v>
       </c>
       <c r="B10" s="23">
         <v>2.5262000000000002</v>
@@ -3631,7 +3813,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="28" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="23">
@@ -3642,7 +3824,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="28" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="23">
@@ -3653,8 +3835,8 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
-        <v>8</v>
+      <c r="A13" s="28" t="s">
+        <v>213</v>
       </c>
       <c r="B13" s="23">
         <v>2.3327999999999998</v>
@@ -3664,7 +3846,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="28" t="s">
         <v>175</v>
       </c>
       <c r="B14" s="23">
@@ -3675,7 +3857,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="28" t="s">
         <v>48</v>
       </c>
       <c r="B15" s="23">
@@ -3686,7 +3868,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="28" t="s">
         <v>82</v>
       </c>
       <c r="B16" s="23">
@@ -3697,8 +3879,8 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
-        <v>6</v>
+      <c r="A17" s="28" t="s">
+        <v>214</v>
       </c>
       <c r="B17" s="23">
         <v>4.165</v>
@@ -3708,7 +3890,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="28" t="s">
         <v>62</v>
       </c>
       <c r="B18" s="23">
@@ -3719,7 +3901,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="28" t="s">
         <v>121</v>
       </c>
       <c r="B19" s="23">
@@ -3730,8 +3912,8 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
-        <v>125</v>
+      <c r="A20" s="28" t="s">
+        <v>215</v>
       </c>
       <c r="B20" s="23">
         <v>1.3784000000000001</v>
@@ -3741,7 +3923,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="28" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="23">
@@ -3752,8 +3934,8 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>33</v>
+      <c r="A22" s="28" t="s">
+        <v>216</v>
       </c>
       <c r="B22" s="23">
         <v>1.1061999999999999</v>
@@ -3763,8 +3945,8 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
-        <v>39</v>
+      <c r="A23" s="28" t="s">
+        <v>217</v>
       </c>
       <c r="B23" s="23">
         <v>7.4756</v>
@@ -3774,7 +3956,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="28" t="s">
         <v>119</v>
       </c>
       <c r="B24" s="23">
@@ -3785,7 +3967,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="28" t="s">
         <v>45</v>
       </c>
       <c r="B25" s="23">
@@ -3796,8 +3978,8 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
-        <v>42</v>
+      <c r="A26" s="28" t="s">
+        <v>218</v>
       </c>
       <c r="B26" s="23">
         <v>1.6597999999999999</v>
@@ -3807,7 +3989,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="28" t="s">
         <v>159</v>
       </c>
       <c r="B27" s="23">
@@ -3818,7 +4000,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="28" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="23">
@@ -3829,8 +4011,8 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
-        <v>176</v>
+      <c r="A29" s="28" t="s">
+        <v>219</v>
       </c>
       <c r="B29" s="23">
         <v>2.9832999999999998</v>
@@ -3840,7 +4022,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="28" t="s">
         <v>149</v>
       </c>
       <c r="B30" s="23">
@@ -3851,7 +4033,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="28" t="s">
         <v>122</v>
       </c>
       <c r="B31" s="23">
@@ -3862,7 +4044,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="28" t="s">
         <v>71</v>
       </c>
       <c r="B32" s="23">
@@ -3873,7 +4055,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="28" t="s">
         <v>114</v>
       </c>
       <c r="B33" s="23">
@@ -3884,8 +4066,8 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="12" t="s">
-        <v>160</v>
+      <c r="A34" s="28" t="s">
+        <v>220</v>
       </c>
       <c r="B34" s="23">
         <v>0.65129999999999999</v>
@@ -3895,8 +4077,8 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="12" t="s">
-        <v>41</v>
+      <c r="A35" s="28" t="s">
+        <v>221</v>
       </c>
       <c r="B35" s="23">
         <v>0.93289999999999995</v>
@@ -3906,7 +4088,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="28" t="s">
         <v>126</v>
       </c>
       <c r="B36" s="23">
@@ -3917,7 +4099,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="12" t="s">
+      <c r="A37" s="28" t="s">
         <v>9</v>
       </c>
       <c r="B37" s="23">
@@ -3928,8 +4110,8 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="12" t="s">
-        <v>127</v>
+      <c r="A38" s="28" t="s">
+        <v>222</v>
       </c>
       <c r="B38" s="23">
         <v>0.99440000000000006</v>
@@ -3939,7 +4121,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="28" t="s">
         <v>150</v>
       </c>
       <c r="B39" s="23">
@@ -3950,7 +4132,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="28" t="s">
         <v>52</v>
       </c>
       <c r="B40" s="23">
@@ -3961,7 +4143,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="28" t="s">
         <v>128</v>
       </c>
       <c r="B41" s="23">
@@ -3972,7 +4154,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="28" t="s">
         <v>161</v>
       </c>
       <c r="B42" s="23">
@@ -3983,8 +4165,8 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="12" t="s">
-        <v>129</v>
+      <c r="A43" s="28" t="s">
+        <v>223</v>
       </c>
       <c r="B43" s="23">
         <v>3.859</v>
@@ -3994,7 +4176,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="12" t="s">
+      <c r="A44" s="28" t="s">
         <v>72</v>
       </c>
       <c r="B44" s="23">
@@ -4005,8 +4187,8 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="12" t="s">
-        <v>34</v>
+      <c r="A45" s="28" t="s">
+        <v>224</v>
       </c>
       <c r="B45" s="23">
         <v>2.0350000000000001</v>
@@ -4016,8 +4198,8 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="12" t="s">
-        <v>130</v>
+      <c r="A46" s="28" t="s">
+        <v>225</v>
       </c>
       <c r="B46" s="23">
         <v>2.4902000000000002</v>
@@ -4027,7 +4209,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="28" t="s">
         <v>27</v>
       </c>
       <c r="B47" s="23">
@@ -4038,8 +4220,8 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="12" t="s">
-        <v>131</v>
+      <c r="A48" s="28" t="s">
+        <v>226</v>
       </c>
       <c r="B48" s="23">
         <v>1.9176</v>
@@ -4049,8 +4231,8 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="12" t="s">
-        <v>23</v>
+      <c r="A49" s="28" t="s">
+        <v>227</v>
       </c>
       <c r="B49" s="23">
         <v>6.4687999999999999</v>
@@ -4060,7 +4242,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="12" t="s">
+      <c r="A50" s="28" t="s">
         <v>64</v>
       </c>
       <c r="B50" s="23">
@@ -4071,8 +4253,8 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="12" t="s">
-        <v>75</v>
+      <c r="A51" s="28" t="s">
+        <v>228</v>
       </c>
       <c r="B51" s="23">
         <v>1.0733999999999999</v>
@@ -4082,8 +4264,8 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="12" t="s">
-        <v>43</v>
+      <c r="A52" s="28" t="s">
+        <v>229</v>
       </c>
       <c r="B52" s="23">
         <v>2.8954</v>
@@ -4093,8 +4275,8 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="12" t="s">
-        <v>17</v>
+      <c r="A53" s="28" t="s">
+        <v>230</v>
       </c>
       <c r="B53" s="23">
         <v>2.4547999999999996</v>
@@ -4104,8 +4286,8 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="12" t="s">
-        <v>132</v>
+      <c r="A54" s="28" t="s">
+        <v>231</v>
       </c>
       <c r="B54" s="23">
         <v>3.4868000000000001</v>
@@ -4115,7 +4297,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="28" t="s">
         <v>2</v>
       </c>
       <c r="B55" s="23">
@@ -4126,7 +4308,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="12" t="s">
+      <c r="A56" s="28" t="s">
         <v>133</v>
       </c>
       <c r="B56" s="23">
@@ -4137,8 +4319,8 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="12" t="s">
-        <v>13</v>
+      <c r="A57" s="28" t="s">
+        <v>232</v>
       </c>
       <c r="B57" s="23">
         <v>1.8694000000000002</v>
@@ -4148,8 +4330,8 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="12" t="s">
-        <v>56</v>
+      <c r="A58" s="28" t="s">
+        <v>233</v>
       </c>
       <c r="B58" s="23">
         <v>2.4620999999999995</v>
@@ -4159,7 +4341,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="12" t="s">
+      <c r="A59" s="28" t="s">
         <v>113</v>
       </c>
       <c r="B59" s="23">
@@ -4170,8 +4352,8 @@
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="12" t="s">
-        <v>177</v>
+      <c r="A60" s="28" t="s">
+        <v>234</v>
       </c>
       <c r="B60" s="23">
         <v>0.73919999999999997</v>
@@ -4181,8 +4363,8 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="12" t="s">
-        <v>20</v>
+      <c r="A61" s="28" t="s">
+        <v>235</v>
       </c>
       <c r="B61" s="23">
         <v>0.99970000000000003</v>
@@ -4192,7 +4374,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="12" t="s">
+      <c r="A62" s="28" t="s">
         <v>100</v>
       </c>
       <c r="B62" s="23">
@@ -4203,7 +4385,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="12" t="s">
+      <c r="A63" s="28" t="s">
         <v>178</v>
       </c>
       <c r="B63" s="23">
@@ -4214,7 +4396,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="12" t="s">
+      <c r="A64" s="28" t="s">
         <v>120</v>
       </c>
       <c r="B64" s="23">
@@ -4225,7 +4407,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="12" t="s">
+      <c r="A65" s="28" t="s">
         <v>102</v>
       </c>
       <c r="B65" s="23">
@@ -4236,7 +4418,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="12" t="s">
+      <c r="A66" s="28" t="s">
         <v>179</v>
       </c>
       <c r="B66" s="23">
@@ -4247,8 +4429,8 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="12" t="s">
-        <v>63</v>
+      <c r="A67" s="28" t="s">
+        <v>236</v>
       </c>
       <c r="B67" s="23">
         <v>1.0301</v>
@@ -4258,8 +4440,8 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="12" t="s">
-        <v>162</v>
+      <c r="A68" s="28" t="s">
+        <v>237</v>
       </c>
       <c r="B68" s="23">
         <v>3.7814999999999999</v>
@@ -4269,8 +4451,8 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="12" t="s">
-        <v>151</v>
+      <c r="A69" s="28" t="s">
+        <v>238</v>
       </c>
       <c r="B69" s="23">
         <v>2.1229</v>
@@ -4280,7 +4462,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="12" t="s">
+      <c r="A70" s="28" t="s">
         <v>134</v>
       </c>
       <c r="B70" s="23">
@@ -4291,7 +4473,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="12" t="s">
+      <c r="A71" s="28" t="s">
         <v>152</v>
       </c>
       <c r="B71" s="23">
@@ -4302,8 +4484,8 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="12" t="s">
-        <v>135</v>
+      <c r="A72" s="28" t="s">
+        <v>239</v>
       </c>
       <c r="B72" s="23">
         <v>2.3643999999999998</v>
@@ -4313,7 +4495,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="12" t="s">
+      <c r="A73" s="28" t="s">
         <v>21</v>
       </c>
       <c r="B73" s="23">
@@ -4324,7 +4506,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="12" t="s">
+      <c r="A74" s="28" t="s">
         <v>73</v>
       </c>
       <c r="B74" s="23">
@@ -4335,7 +4517,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="17" t="s">
+      <c r="A75" s="28" t="s">
         <v>61</v>
       </c>
       <c r="B75" s="23">
@@ -4346,8 +4528,8 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
-        <v>180</v>
+      <c r="A76" s="28" t="s">
+        <v>240</v>
       </c>
       <c r="B76" s="23">
         <v>0.62070000000000003</v>
@@ -4357,8 +4539,8 @@
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="s">
-        <v>40</v>
+      <c r="A77" s="28" t="s">
+        <v>241</v>
       </c>
       <c r="B77" s="23">
         <v>0.42270000000000002</v>
@@ -4368,7 +4550,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="28" t="s">
         <v>163</v>
       </c>
       <c r="B78" s="23">
@@ -4379,19 +4561,19 @@
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B79" s="26" t="s">
-        <v>204</v>
-      </c>
-      <c r="C79" s="26" t="s">
-        <v>204</v>
+      <c r="A79" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="B79" s="26">
+        <v>0</v>
+      </c>
+      <c r="C79" s="26">
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
-        <v>60</v>
+      <c r="A80" s="28" t="s">
+        <v>243</v>
       </c>
       <c r="B80" s="23">
         <v>0.8397</v>
@@ -4401,7 +4583,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="28" t="s">
         <v>181</v>
       </c>
       <c r="B81" s="23">
@@ -4412,7 +4594,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="2" t="s">
+      <c r="A82" s="28" t="s">
         <v>115</v>
       </c>
       <c r="B82" s="23">
@@ -4423,7 +4605,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" s="2" t="s">
+      <c r="A83" s="28" t="s">
         <v>199</v>
       </c>
       <c r="B83" s="23">
@@ -4434,7 +4616,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" s="2" t="s">
+      <c r="A84" s="28" t="s">
         <v>153</v>
       </c>
       <c r="B84" s="23">
@@ -4445,7 +4627,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="s">
+      <c r="A85" s="28" t="s">
         <v>58</v>
       </c>
       <c r="B85" s="23">
@@ -4456,8 +4638,8 @@
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
-        <v>50</v>
+      <c r="A86" s="28" t="s">
+        <v>244</v>
       </c>
       <c r="B86" s="23">
         <v>1.3852</v>
@@ -4467,7 +4649,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" s="2" t="s">
+      <c r="A87" s="28" t="s">
         <v>136</v>
       </c>
       <c r="B87" s="23">
@@ -4478,7 +4660,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" s="2" t="s">
+      <c r="A88" s="28" t="s">
         <v>137</v>
       </c>
       <c r="B88" s="23">
@@ -4489,8 +4671,8 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" s="2" t="s">
-        <v>138</v>
+      <c r="A89" s="28" t="s">
+        <v>245</v>
       </c>
       <c r="B89" s="23">
         <v>0.50360000000000005</v>
@@ -4500,8 +4682,8 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" s="2" t="s">
-        <v>165</v>
+      <c r="A90" s="28" t="s">
+        <v>246</v>
       </c>
       <c r="B90" s="23">
         <v>0.69159999999999999</v>
@@ -4511,8 +4693,8 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" s="20" t="s">
-        <v>80</v>
+      <c r="A91" s="28" t="s">
+        <v>247</v>
       </c>
       <c r="B91" s="23">
         <v>1.2076</v>
@@ -4522,7 +4704,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" s="12" t="s">
+      <c r="A92" s="28" t="s">
         <v>99</v>
       </c>
       <c r="B92" s="23">
@@ -4533,8 +4715,8 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" s="12" t="s">
-        <v>123</v>
+      <c r="A93" s="28" t="s">
+        <v>248</v>
       </c>
       <c r="B93" s="23">
         <v>1.1486999999999998</v>
@@ -4544,8 +4726,8 @@
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" s="12" t="s">
-        <v>139</v>
+      <c r="A94" s="28" t="s">
+        <v>249</v>
       </c>
       <c r="B94" s="23">
         <v>0.52210000000000001</v>
@@ -4555,8 +4737,8 @@
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" s="12" t="s">
-        <v>140</v>
+      <c r="A95" s="28" t="s">
+        <v>250</v>
       </c>
       <c r="B95" s="23">
         <v>0.2366</v>
@@ -4566,7 +4748,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="12" t="s">
+      <c r="A96" s="28" t="s">
         <v>141</v>
       </c>
       <c r="B96" s="23">
@@ -4577,7 +4759,7 @@
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="12" t="s">
+      <c r="A97" s="28" t="s">
         <v>164</v>
       </c>
       <c r="B97" s="23">
@@ -4588,8 +4770,8 @@
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="12" t="s">
-        <v>142</v>
+      <c r="A98" s="28" t="s">
+        <v>251</v>
       </c>
       <c r="B98" s="23">
         <v>1.5547999999999997</v>
@@ -4599,7 +4781,7 @@
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="12" t="s">
+      <c r="A99" s="28" t="s">
         <v>92</v>
       </c>
       <c r="B99" s="23">
@@ -4610,8 +4792,8 @@
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="12" t="s">
-        <v>87</v>
+      <c r="A100" s="28" t="s">
+        <v>252</v>
       </c>
       <c r="B100" s="23">
         <v>2.3679000000000001</v>
@@ -4621,7 +4803,7 @@
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="12" t="s">
+      <c r="A101" s="28" t="s">
         <v>154</v>
       </c>
       <c r="B101" s="23">
@@ -4632,7 +4814,7 @@
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="12" t="s">
+      <c r="A102" s="28" t="s">
         <v>155</v>
       </c>
       <c r="B102" s="23">
@@ -4643,7 +4825,7 @@
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" s="12" t="s">
+      <c r="A103" s="28" t="s">
         <v>166</v>
       </c>
       <c r="B103" s="23">
@@ -4654,7 +4836,7 @@
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="12" t="s">
+      <c r="A104" s="28" t="s">
         <v>167</v>
       </c>
       <c r="B104" s="23">
@@ -4665,7 +4847,7 @@
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" s="12" t="s">
+      <c r="A105" s="28" t="s">
         <v>143</v>
       </c>
       <c r="B105" s="23">
@@ -4676,7 +4858,7 @@
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="12" t="s">
+      <c r="A106" s="28" t="s">
         <v>105</v>
       </c>
       <c r="B106" s="23">
@@ -4687,7 +4869,7 @@
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" s="12" t="s">
+      <c r="A107" s="28" t="s">
         <v>144</v>
       </c>
       <c r="B107" s="23">
@@ -4698,7 +4880,7 @@
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" s="12" t="s">
+      <c r="A108" s="28" t="s">
         <v>156</v>
       </c>
       <c r="B108" s="23">
@@ -4709,7 +4891,7 @@
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" s="12" t="s">
+      <c r="A109" s="28" t="s">
         <v>168</v>
       </c>
       <c r="B109" s="23">
@@ -4720,8 +4902,8 @@
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" s="12" t="s">
-        <v>96</v>
+      <c r="A110" s="28" t="s">
+        <v>253</v>
       </c>
       <c r="B110" s="23">
         <v>1.5344</v>
@@ -4731,8 +4913,8 @@
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" s="12" t="s">
-        <v>107</v>
+      <c r="A111" s="28" t="s">
+        <v>254</v>
       </c>
       <c r="B111" s="23">
         <v>3.6463000000000001</v>
@@ -4742,7 +4924,7 @@
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" s="12" t="s">
+      <c r="A112" s="28" t="s">
         <v>14</v>
       </c>
       <c r="B112" s="23">
@@ -4753,8 +4935,8 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" s="12" t="s">
-        <v>94</v>
+      <c r="A113" s="28" t="s">
+        <v>255</v>
       </c>
       <c r="B113" s="23">
         <v>0.25</v>
@@ -4764,8 +4946,8 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" s="12" t="s">
-        <v>182</v>
+      <c r="A114" s="28" t="s">
+        <v>256</v>
       </c>
       <c r="B114" s="23">
         <v>1.3353999999999999</v>
@@ -4775,7 +4957,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" s="12" t="s">
+      <c r="A115" s="28" t="s">
         <v>169</v>
       </c>
       <c r="B115" s="23">
@@ -4786,8 +4968,8 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" s="12" t="s">
-        <v>85</v>
+      <c r="A116" s="28" t="s">
+        <v>257</v>
       </c>
       <c r="B116" s="23">
         <v>0.45450000000000002</v>
@@ -4797,7 +4979,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117" s="12" t="s">
+      <c r="A117" s="28" t="s">
         <v>118</v>
       </c>
       <c r="B117" s="23">
@@ -4808,7 +4990,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" s="12" t="s">
+      <c r="A118" s="28" t="s">
         <v>117</v>
       </c>
       <c r="B118" s="23">
@@ -4819,8 +5001,8 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" s="12" t="s">
-        <v>89</v>
+      <c r="A119" s="28" t="s">
+        <v>258</v>
       </c>
       <c r="B119" s="23">
         <v>1.9377</v>
@@ -4830,8 +5012,8 @@
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" s="12" t="s">
-        <v>145</v>
+      <c r="A120" s="28" t="s">
+        <v>259</v>
       </c>
       <c r="B120" s="23">
         <v>0.33189999999999997</v>
@@ -4841,8 +5023,8 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121" s="12" t="s">
-        <v>78</v>
+      <c r="A121" s="28" t="s">
+        <v>260</v>
       </c>
       <c r="B121" s="23">
         <v>0.52239999999999998</v>
@@ -4852,7 +5034,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122" s="12" t="s">
+      <c r="A122" s="28" t="s">
         <v>116</v>
       </c>
       <c r="B122" s="23">
@@ -4863,7 +5045,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" s="12" t="s">
+      <c r="A123" s="28" t="s">
         <v>146</v>
       </c>
       <c r="B123" s="23">
@@ -4874,8 +5056,8 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A124" s="12" t="s">
-        <v>95</v>
+      <c r="A124" s="28" t="s">
+        <v>261</v>
       </c>
       <c r="B124" s="23">
         <v>1.1252</v>
@@ -4885,8 +5067,8 @@
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" s="12" t="s">
-        <v>147</v>
+      <c r="A125" s="28" t="s">
+        <v>262</v>
       </c>
       <c r="B125" s="23">
         <v>0.38109999999999999</v>
@@ -4896,8 +5078,8 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" s="12" t="s">
-        <v>148</v>
+      <c r="A126" s="28" t="s">
+        <v>263</v>
       </c>
       <c r="B126" s="23">
         <v>1.2757000000000001</v>
@@ -4907,7 +5089,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A127" s="12" t="s">
+      <c r="A127" s="28" t="s">
         <v>170</v>
       </c>
       <c r="B127" s="23">
@@ -4918,7 +5100,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128" s="12" t="s">
+      <c r="A128" s="28" t="s">
         <v>183</v>
       </c>
       <c r="B128" s="23">
@@ -4929,7 +5111,7 @@
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" s="12" t="s">
+      <c r="A129" s="28" t="s">
         <v>184</v>
       </c>
       <c r="B129" s="23">
@@ -4940,7 +5122,7 @@
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130" s="12" t="s">
+      <c r="A130" s="28" t="s">
         <v>157</v>
       </c>
       <c r="B130" s="23">
@@ -4950,8 +5132,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="13" t="s">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="28" t="s">
         <v>91</v>
       </c>
       <c r="B131" s="23">

</xml_diff>